<commit_message>
adicionando metodo gerenciamento de alertas para organizar o program
</commit_message>
<xml_diff>
--- a/RPA_Teste/DataBase/Input.xlsx
+++ b/RPA_Teste/DataBase/Input.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA\Finanças\Rpa_Challenge\RPA_Teste\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1B871E-2B3D-4475-8B47-24B34355F933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B12AC1-DF86-4636-88AC-9B52DAD5375B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10770" yWindow="3465" windowWidth="13560" windowHeight="9555" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acoes" sheetId="1" r:id="rId1"/>
     <sheet name="Fundos" sheetId="2" r:id="rId2"/>
     <sheet name="Configs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>NOME</t>
   </si>
@@ -95,6 +95,9 @@
     <t>BBSE3</t>
   </si>
   <si>
+    <t>BBDC4</t>
+  </si>
+  <si>
     <t>KNSC11</t>
   </si>
   <si>
@@ -134,9 +137,6 @@
     <t>VINO11</t>
   </si>
   <si>
-    <t>BBDC4</t>
-  </si>
-  <si>
     <t>ETAPA</t>
   </si>
   <si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>ENVIAR ALERTA PRECOS</t>
+  </si>
+  <si>
+    <t>ENVIAR LOG MENSAGEM</t>
   </si>
 </sst>
 </file>
@@ -212,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -238,6 +241,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,7 +525,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView zoomScale="94" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A5" sqref="A5 A4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,8 +572,8 @@
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
+      <c r="B4" s="2">
+        <v>34</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -679,7 +683,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -701,7 +705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB79D21-E832-4875-A540-96CDC26ACCCD}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -725,10 +729,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -736,10 +740,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -747,7 +751,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -758,7 +762,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2">
         <v>75</v>
@@ -769,7 +773,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -780,7 +784,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -791,7 +795,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2">
         <v>83</v>
@@ -802,10 +806,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
@@ -813,7 +817,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2">
         <v>95</v>
@@ -825,7 +829,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" s="2">
         <v>7</v>
@@ -848,10 +852,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49AE673B-CCAC-45C7-AC1A-067FB96F1582}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +864,7 @@
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>36</v>
       </c>
@@ -868,29 +872,40 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
atualizando formatacao documento input
</commit_message>
<xml_diff>
--- a/RPA_Teste/DataBase/Input.xlsx
+++ b/RPA_Teste/DataBase/Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA\Finanças\Rpa_Challenge\RPA_Teste\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B12AC1-DF86-4636-88AC-9B52DAD5375B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF2DF29-76F1-4224-9604-6DA1DAC2AD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10770" yWindow="3465" windowWidth="13560" windowHeight="9555" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,16 +215,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -237,11 +234,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,7 +522,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView zoomScale="94" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5 A4:B5"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,14 +532,14 @@
     <col min="3" max="3" width="18.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -706,7 +703,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,22 +713,22 @@
     <col min="3" max="3" width="18.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="2">
@@ -828,7 +825,7 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="2">
@@ -855,7 +852,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,19 +861,19 @@
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionando modalidade de envio de log por word
</commit_message>
<xml_diff>
--- a/RPA_Teste/DataBase/Input.xlsx
+++ b/RPA_Teste/DataBase/Input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA\Finanças\Rpa_Challenge\RPA_Teste\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF2DF29-76F1-4224-9604-6DA1DAC2AD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC063F63-24B6-4EFE-8FA2-FFA8C9480979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10770" yWindow="3465" windowWidth="13560" windowHeight="9555" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acoes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>NOME</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>ENVIAR LOG MENSAGEM</t>
+  </si>
+  <si>
+    <t>ENVIAR LOG WORD</t>
   </si>
 </sst>
 </file>
@@ -852,7 +855,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,6 +904,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F15" s="1"/>
     </row>

</xml_diff>